<commit_message>
feat: Replace Amazon image URL suffixes with _SL1664_ and ensure uniqueness
- Updated `filter_amazon_urls` function:
  - Replaces allowed suffixes (`_SL1200_`, `_SL1500_`, `_SY355_`) with `_SL1664_`.
  - Ensures all modified URLs are unique using a set.
  - Converts the set back to a list for the final output.

- Improved efficiency:
  - Stops checking suffixes once a match is found using `break`.
</commit_message>
<xml_diff>
--- a/data/output_scraper_results.xlsx
+++ b/data/output_scraper_results.xlsx
@@ -7,7 +7,9 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="All Details Laptop" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Flipkart Laptop Details" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="To Be Checked Again" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Amazon Laptop Details" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BK5"/>
+  <dimension ref="A1:BJ3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -741,11 +743,6 @@
       </c>
       <c r="BJ1" s="1" t="inlineStr">
         <is>
-          <t>HDMI Port</t>
-        </is>
-      </c>
-      <c r="BK1" s="1" t="inlineStr">
-        <is>
           <t>Processor Generation</t>
         </is>
       </c>
@@ -788,7 +785,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>['https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/v/t/b/-original-imagvkpfbpgzzqfe.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/a/i/i/-original-imagzk3kfk6bktha.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/3/j/a/z2-493-thin-and-light-laptop-acer-original-imagr6yjpmhhmpvm.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/d/u/y/-original-imagzk3kukhhjdhq.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/x/h/l/-original-imagzk3kcpg6fzxf.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/l/u/v/z2-493-thin-and-light-laptop-acer-original-imagr6yjuvhjntcb.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/o/x/n/-original-imagzk3kuu8kduxk.jpeg?q=100&amp;crop=false']</t>
+          <t>['https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/v/t/b/-original-imagvkpfbpgzzqfe.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/3/j/a/z2-493-thin-and-light-laptop-acer-original-imagr6yjpmhhmpvm.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/o/x/n/-original-imagzk3kuu8kduxk.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/x/h/l/-original-imagzk3kcpg6fzxf.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/d/u/y/-original-imagzk3kukhhjdhq.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/l/u/v/z2-493-thin-and-light-laptop-acer-original-imagr6yjuvhjntcb.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/a/i/i/-original-imagzk3kfk6bktha.jpeg?q=100&amp;crop=false']</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -1046,48 +1043,46 @@
           <t>1 Year</t>
         </is>
       </c>
-      <c r="BJ2" t="inlineStr"/>
-      <c r="BK2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Acer Aspire 3 Intel Celeron Dual Core N4500 - (8 GB/512 GB SSD/Windows 11 Home) A324-45 Thin and Light Laptop  (14 Inch, Pure Silver, 1.3 Kg)</t>
+          <t>Acer Aspire 3 Spin 14 Intel Core i3 13th Gen N305 - (8 GB/512 GB SSD/Windows 11 Home) A3SP14-31PT-3554 Thin and Light Laptop  (14 inch, Silver, 1.54 Kg, With MS Office)</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>₹20,990</t>
+          <t>₹40,100</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>₹32,999</t>
+          <t>₹55,140</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Thin, light, and powerful laptop with an HD display and Intel Core Celeron processor. Features an integrated camera privacy shutter and a versatile 180-degree hinge.</t>
+          <t>In the world of laptops, where innovation meets functionality, the Acer Aspire 3 Spin 14 emerges as a versatile virtuoso, transcending the boundaries of conventional computing. With a design that seamlessly blends thinness, lightness, and versatility, this 2-in-1 convertible laptop is not just a device; it's a gateway to a world where your ideas come to life. It's not just a laptop; it's an experience that unfolds with every flip, every touch, and every task. As you delve into the thin, light, and versatile world of this convertible laptop, you realize it's not just a device; it's a companion that enhances your journey through the digital realm. Welcome to a new era of computing; welcome to the Acer Aspire 3 Spin 14 experience.</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Acer Aspire 3 Intel Celeron Dual Core N4500 - (8 GB/512 GB SSD/Windows 11 Home) A324-45 Thin and Light Laptop Rs.32999  Price in India - Buy Acer Aspire 3 Intel Celeron Dual Core N4500 - (8 GB/512 GB SSD/Windows 11 Home) A324-45 Thin and Light Laptop Pure Silver Online - Acer : Flipkart.com</t>
+          <t>Acer Aspire 3 Spin 14 Intel Core i3 13th Gen N305 - (8 GB/512 GB SSD/Windows 11 Home) A3SP14-31PT-3554 Thin and Light Laptop Rs.55140  Price in India - Buy Acer Aspire 3 Spin 14 Intel Core i3 13th Gen N305 - (8 GB/512 GB SSD/Windows 11 Home) A3SP14-31PT-3554 Thin and Light Laptop Silver Online - Acer : Flipkart.com</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Acer Aspire 3 Intel Celeron Dual Core N4500 - (8 GB/512 GB SSD/Windows 11 Home) A324-45 Thin and Light Laptop Price, Acer Aspire 3 Intel Celeron Dual Core N4500 - (8 GB/512 GB SSD/Windows 11 Home) A324-45 Thin and Light Laptop Specifications, Acer Aspire 3 Intel Celeron Dual Core N4500 - (8 GB/512 GB SSD/Windows 11 Home) A324-45 Thin and Light Laptop Features</t>
+          <t>Acer Aspire 3 Spin 14 Intel Core i3 13th Gen N305 - (8 GB/512 GB SSD/Windows 11 Home) A3SP14-31PT-3554 Thin and Light Laptop Price, Acer Aspire 3 Spin 14 Intel Core i3 13th Gen N305 - (8 GB/512 GB SSD/Windows 11 Home) A3SP14-31PT-3554 Thin and Light Laptop Specifications, Acer Aspire 3 Spin 14 Intel Core i3 13th Gen N305 - (8 GB/512 GB SSD/Windows 11 Home) A3SP14-31PT-3554 Thin and Light Laptop Features</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Buy Acer Aspire 3 Intel Celeron Dual Core N4500 - (8 GB/512 GB SSD/Windows 11 Home) A324-45 Thin and Light Laptop Online For Rs.32999 , Also get Acer Aspire 3 Intel Celeron Dual Core N4500 - (8 GB/512 GB SSD/Windows 11 Home) A324-45 Thin and Light Laptop Specifications &amp; Features. Only Genuine Products. 30 Day Replacement Guarantee. Free Shipping. Cash On Delivery!</t>
+          <t>Buy Acer Aspire 3 Spin 14 Intel Core i3 13th Gen N305 - (8 GB/512 GB SSD/Windows 11 Home) A3SP14-31PT-3554 Thin and Light Laptop Online For Rs.55140 , Also get Acer Aspire 3 Spin 14 Intel Core i3 13th Gen N305 - (8 GB/512 GB SSD/Windows 11 Home) A3SP14-31PT-3554 Thin and Light Laptop Specifications &amp; Features. Only Genuine Products. 30 Day Replacement Guarantee. Free Shipping. Cash On Delivery!</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>['https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/v/i/t/a324-45-thin-and-light-laptop-acer-original-imah6gfd7spzq4w2.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/p/c/b/-original-imah2z85gzvpqdy3.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/m/l/4/-original-imah5q7sszgwr7ff.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/9/f/v/a324-45-thin-and-light-laptop-acer-original-imah6gfdzgknkz7y.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/x/a/a/a324-45-thin-and-light-laptop-acer-original-imah6gfdmyzghr2g.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/d/i/q/a324-45-thin-and-light-laptop-acer-original-imah6gfdswqqhgzv.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/k/p/v/a324-45-thin-and-light-laptop-acer-original-imah6gfdwgay6yfx.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/allinone-desktop/f/i/q/-original-imagrym4vdpjmtnc.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/s/u/i/a324-45-thin-and-light-laptop-acer-original-imah6gfdarxehb3z.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/8/p/o/a324-45-thin-and-light-laptop-acer-original-imah6gfdagzdtyzg.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/i/j/l/a324-45-thin-and-light-laptop-acer-original-imah6gfdkf2m5rjf.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/s/j/0/a324-45-thin-and-light-laptop-acer-original-imah6gfdmbpwpgga.jpeg?q=100&amp;crop=false']</t>
+          <t>['https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/i/2/e/a3sp14-31pt-thin-and-light-laptop-acer-original-imah4bj3zty7uwzt.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/i/n/p/a3sp14-31pt-thin-and-light-laptop-acer-original-imah4bj3jtt5ht8g.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/g/f/r/a3sp14-31pt-thin-and-light-laptop-acer-original-imah4bj3b5edadhw.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/d/p/j/-original-imagwkaymfh66hw3.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/p/j/o/a3sp14-31pt-thin-and-light-laptop-acer-original-imah4bj3vxnbzuzx.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/f/w/y/a3sp14-31pt-thin-and-light-laptop-acer-original-imah4bj3ggcejgxd.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/z/m/n/a3sp14-31pt-thin-and-light-laptop-acer-original-imah4bj3v9f9uqff.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/x/u/3/a3sp14-31pt-thin-and-light-laptop-acer-original-imah4bj3kzhphypa.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/q/j/a/a3sp14-31pt-thin-and-light-laptop-acer-original-imah4bj3nvfzgk9g.jpeg?q=100&amp;crop=false']</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -1097,714 +1092,852 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>A324-45</t>
+          <t>A3SP14-31PT-3554</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>UN.342SI.004</t>
+          <t>NX.KENSI.004</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>A324-45</t>
+          <t>A3SP14-31PT</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
+          <t>Aspire 3 Spin 14</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>Silver</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>Thin and Light Laptop</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>Processing &amp; Multitasking</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>Intel</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>Core i3</t>
+        </is>
+      </c>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>512 GB</t>
+        </is>
+      </c>
+      <c r="X3" t="inlineStr">
+        <is>
+          <t>8 GB</t>
+        </is>
+      </c>
+      <c r="Y3" t="inlineStr">
+        <is>
+          <t>LPDDR5</t>
+        </is>
+      </c>
+      <c r="Z3" t="inlineStr">
+        <is>
+          <t>N305</t>
+        </is>
+      </c>
+      <c r="AA3" t="inlineStr">
+        <is>
+          <t>Max Frequency Up to 3.8 GHz</t>
+        </is>
+      </c>
+      <c r="AD3" t="inlineStr">
+        <is>
+          <t>Intel Integrated UHD</t>
+        </is>
+      </c>
+      <c r="AF3" t="inlineStr">
+        <is>
+          <t>SSD</t>
+        </is>
+      </c>
+      <c r="AH3" t="inlineStr">
+        <is>
+          <t>Windows 11 Home</t>
+        </is>
+      </c>
+      <c r="AM3" t="inlineStr">
+        <is>
+          <t>1 x USB Type-C port with DC-in, 2 x USB 3.2 port</t>
+        </is>
+      </c>
+      <c r="AN3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AO3" t="inlineStr">
+        <is>
+          <t>35.56 cm (14 inch)</t>
+        </is>
+      </c>
+      <c r="AP3" t="inlineStr">
+        <is>
+          <t>1920 x 1200 Pixel</t>
+        </is>
+      </c>
+      <c r="AQ3" t="inlineStr">
+        <is>
+          <t>Full HD, TFT, LCD</t>
+        </is>
+      </c>
+      <c r="AR3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AS3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AT3" t="inlineStr">
+        <is>
+          <t>WIFI6+BT - 1x1 AX</t>
+        </is>
+      </c>
+      <c r="AU3" t="inlineStr">
+        <is>
+          <t>v5.2</t>
+        </is>
+      </c>
+      <c r="AW3" t="inlineStr">
+        <is>
+          <t>319.8 x 227.9 x 18.9 mm</t>
+        </is>
+      </c>
+      <c r="AX3" t="inlineStr">
+        <is>
+          <t>1.54 Kg</t>
+        </is>
+      </c>
+      <c r="AY3" t="inlineStr">
+        <is>
+          <t>Not Available</t>
+        </is>
+      </c>
+      <c r="AZ3" t="inlineStr">
+        <is>
+          <t>T-Type HD camera with 1280 x 720 resolution and 720p HD video at 30 fps with Temporal Noise Reduction</t>
+        </is>
+      </c>
+      <c r="BB3" t="inlineStr">
+        <is>
+          <t>80-/81-/84-key Acer keyboard layout with international language support including indicators of CapsLock and F4/Microphone mute</t>
+        </is>
+      </c>
+      <c r="BC3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BE3" t="inlineStr">
+        <is>
+          <t>1 Year Onsite Warranty</t>
+        </is>
+      </c>
+      <c r="BF3" t="inlineStr">
+        <is>
+          <t>Onsite</t>
+        </is>
+      </c>
+      <c r="BG3" t="inlineStr">
+        <is>
+          <t>Manufacturing Defects</t>
+        </is>
+      </c>
+      <c r="BH3" t="inlineStr">
+        <is>
+          <t>Physical Damage</t>
+        </is>
+      </c>
+      <c r="BJ3" t="inlineStr">
+        <is>
+          <t>13th Gen</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Product Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Model Name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Color</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Category</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Link</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>91 Link</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>acer</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>aspire 3 intel celeron dual core n4500 8 gb 512 gb ssb</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Laptop</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>https://www.amazon.in/Acer-Celeron-Processor-LPDDR4X-A325-45/dp/B0D7PYTTGH</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>https://www.91mobiles.com/acer-a325-45-un-344si-004-intel-celeron-dual-core-8-gb-512-gb-windows-11-laptop-price-in-india-163983</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:BC2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Product Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Offer Price</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>MRP</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Images</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Brand</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Model</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Series</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Thickness</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Dimensions (WxDxH)</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Weight</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Colour(s)</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Operating System</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Operating System Type</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Display Size</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Display Resolution</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Pixel Density</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Display Features</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Touchscreen</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>Aspect Ratio</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>Processor</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Number of Cores</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>Graphic Processor</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>Capacity</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>RAM type</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>Memory Slots</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>Expandable Memory</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>Memory Layout</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>SSD Capacity</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>Battery Cell</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>Battery type</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>Power Supply</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>Battery Capacity</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>Wireless LAN</t>
+        </is>
+      </c>
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t>Wi-Fi Version</t>
+        </is>
+      </c>
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>Bluetooth</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
+          <t>Bluetooth Version</t>
+        </is>
+      </c>
+      <c r="AM1" s="1" t="inlineStr">
+        <is>
+          <t>HDMI Ports</t>
+        </is>
+      </c>
+      <c r="AN1" s="1" t="inlineStr">
+        <is>
+          <t>USB Type C</t>
+        </is>
+      </c>
+      <c r="AO1" s="1" t="inlineStr">
+        <is>
+          <t>SD Card Reader</t>
+        </is>
+      </c>
+      <c r="AP1" s="1" t="inlineStr">
+        <is>
+          <t>Headphone Jack</t>
+        </is>
+      </c>
+      <c r="AQ1" s="1" t="inlineStr">
+        <is>
+          <t>Microphone Jack</t>
+        </is>
+      </c>
+      <c r="AR1" s="1" t="inlineStr">
+        <is>
+          <t>VGA Port</t>
+        </is>
+      </c>
+      <c r="AS1" s="1" t="inlineStr">
+        <is>
+          <t>Webcam</t>
+        </is>
+      </c>
+      <c r="AT1" s="1" t="inlineStr">
+        <is>
+          <t>Video Recording</t>
+        </is>
+      </c>
+      <c r="AU1" s="1" t="inlineStr">
+        <is>
+          <t>Speakers</t>
+        </is>
+      </c>
+      <c r="AV1" s="1" t="inlineStr">
+        <is>
+          <t>In-built Microphone</t>
+        </is>
+      </c>
+      <c r="AW1" s="1" t="inlineStr">
+        <is>
+          <t>Microphone Type</t>
+        </is>
+      </c>
+      <c r="AX1" s="1" t="inlineStr">
+        <is>
+          <t>Pointing Device</t>
+        </is>
+      </c>
+      <c r="AY1" s="1" t="inlineStr">
+        <is>
+          <t>Keyboard</t>
+        </is>
+      </c>
+      <c r="AZ1" s="1" t="inlineStr">
+        <is>
+          <t>Face Recognition</t>
+        </is>
+      </c>
+      <c r="BA1" s="1" t="inlineStr">
+        <is>
+          <t>Warranty</t>
+        </is>
+      </c>
+      <c r="BB1" s="1" t="inlineStr">
+        <is>
+          <t>Lockport</t>
+        </is>
+      </c>
+      <c r="BC1" s="1" t="inlineStr">
+        <is>
+          <t>Sales Package</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Acer Aspire 3 Laptop Intel Core Celeron N4500 Processor Laptop (8 GB LPDDR4X SDRAM/512 GB SSD/Win11 Home/38 WHR/HD Webcam) A325-45 with 39.63 cm (15.6") HD Display, Pure Silver, 1.5 KG</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>21990</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>33999</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Processor : Whether you're at home, school, or work, get all the performance you need with the latest Intel Celeron N4500 Processor @ 1.10GHz ( 2 Cores, 4M Cache, up to 2.80 GHz); maintaining order and keeping your apps running consistently and smoothly. Performance : 8GB LPDDR4X RAM for full-power multitasking; 512GB SSD; Thisthin and light laptop offers a good experience for watching videos, browsing the web, remote work, or study from home. Display : 15.6-inch HD 1366 x 768 resolution display keeps images and videos stunning while the narrow border offers-up more viewable space. To protect user’s eyes from harmful blue light, it also includes Acer BlueLightShield. Wireless Connectivity : Dual band Wi-Fi 5 (802.11ac) provides fast internet access. For enhanced video calls this laptop also includes and optimized camera and microphones. Plenty of Ports : Flexible connectivity options through USB 3.0 ports. Users can also connect an external display through the HDMI port.</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>['https://m.media-amazon.com/images/I/61qlqvTsocL._SL1664_.jpg', 'https://m.media-amazon.com/images/I/71Mwxs8TX+L._SL1664_.jpg', 'https://m.media-amazon.com/images/I/71p+Rn+JgbL._SL1664_.jpg', 'https://m.media-amazon.com/images/I/71W6EmfwI-L._SL1664_.jpg', 'https://m.media-amazon.com/images/I/71MllJzfDfL._SL1664_.jpg', 'https://m.media-amazon.com/images/I/71V25H7JYBL._SL1664_.jpg']</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Acer Aspire 3 A325-45 (UN.344SI.004) Laptop (Intel Celeron Dual Core/8 GB/512 GB SSD/Windows 11)</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Acer</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>A325-45 (UN.344SI.004)</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
           <t>Aspire 3</t>
         </is>
       </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>Pure Silver</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>Thin and Light Laptop</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>Processing &amp; Multitasking</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr">
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>17.7 Millimeter thickness</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>357.4 x 228 x 17.7  mm</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>1.5 Kg weight</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>Silver</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>Windows 11 Home Basic</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>64-bit</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>15.6 Inches (39.62 cm)</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>1366 x 768 Pixels</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>100 ppi</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>TN Display With HD
+Acer ComfyView LED-Backlit TFT LCD
+Ultra-Slim Design
+Mercury Free
+Environment Friendly</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>16:9</t>
+        </is>
+      </c>
+      <c r="V2" t="inlineStr">
+        <is>
+          <t>Intel Celeron Dual Core - N4500</t>
+        </is>
+      </c>
+      <c r="W2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="X2" t="inlineStr">
+        <is>
+          <t>Intel UHD</t>
+        </is>
+      </c>
+      <c r="Y2" t="inlineStr">
+        <is>
+          <t>8 GB</t>
+        </is>
+      </c>
+      <c r="Z2" t="inlineStr">
+        <is>
+          <t>LPDDR4X</t>
+        </is>
+      </c>
+      <c r="AA2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AB2" t="inlineStr">
+        <is>
+          <t>8 GB</t>
+        </is>
+      </c>
+      <c r="AC2" t="inlineStr">
+        <is>
+          <t>1*8 Gigabyte</t>
+        </is>
+      </c>
+      <c r="AD2" t="inlineStr">
+        <is>
+          <t>512 GB</t>
+        </is>
+      </c>
+      <c r="AE2" t="inlineStr">
+        <is>
+          <t>2 Cell</t>
+        </is>
+      </c>
+      <c r="AF2" t="inlineStr">
+        <is>
+          <t>Li-Ion</t>
+        </is>
+      </c>
+      <c r="AG2" t="inlineStr">
         <is>
           <t>24 W</t>
         </is>
       </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>2 cell</t>
-        </is>
-      </c>
-      <c r="S3" t="inlineStr">
+      <c r="AH2" t="inlineStr">
+        <is>
+          <t>38 WHrs</t>
+        </is>
+      </c>
+      <c r="AI2" t="inlineStr">
+        <is>
+          <t>802.11 a/b/g/n/ac</t>
+        </is>
+      </c>
+      <c r="AJ2" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="AK2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AL2" t="inlineStr">
+        <is>
+          <t>5.0</t>
+        </is>
+      </c>
+      <c r="AM2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AN2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AO2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AP2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AQ2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AR2" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t>Intel</t>
-        </is>
-      </c>
-      <c r="U3" t="inlineStr">
-        <is>
-          <t>Celeron Dual Core</t>
-        </is>
-      </c>
-      <c r="V3" t="inlineStr">
+      <c r="AS2" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="W3" t="inlineStr">
-        <is>
-          <t>512 GB</t>
-        </is>
-      </c>
-      <c r="X3" t="inlineStr">
-        <is>
-          <t>8 GB</t>
-        </is>
-      </c>
-      <c r="Y3" t="inlineStr">
-        <is>
-          <t>LPDDR4X</t>
-        </is>
-      </c>
-      <c r="Z3" t="inlineStr">
-        <is>
-          <t>N4500</t>
-        </is>
-      </c>
-      <c r="AA3" t="inlineStr"/>
-      <c r="AB3" t="inlineStr"/>
-      <c r="AC3" t="inlineStr"/>
-      <c r="AD3" t="inlineStr">
-        <is>
-          <t>Intel Integrated UHD</t>
-        </is>
-      </c>
-      <c r="AE3" t="inlineStr"/>
-      <c r="AF3" t="inlineStr">
-        <is>
-          <t>SSD</t>
-        </is>
-      </c>
-      <c r="AG3" t="inlineStr"/>
-      <c r="AH3" t="inlineStr">
-        <is>
-          <t>Windows 11 Home</t>
-        </is>
-      </c>
-      <c r="AI3" t="inlineStr"/>
-      <c r="AJ3" t="inlineStr"/>
-      <c r="AK3" t="inlineStr"/>
-      <c r="AL3" t="inlineStr"/>
-      <c r="AM3" t="inlineStr">
-        <is>
-          <t>USB 3.0 ports</t>
-        </is>
-      </c>
-      <c r="AN3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="AO3" t="inlineStr">
-        <is>
-          <t>35.56 cm (14 Inch)</t>
-        </is>
-      </c>
-      <c r="AP3" t="inlineStr">
-        <is>
-          <t>1366 x 768 Pixel</t>
-        </is>
-      </c>
-      <c r="AQ3" t="inlineStr">
-        <is>
-          <t>HD</t>
-        </is>
-      </c>
-      <c r="AR3" t="inlineStr">
+      <c r="AT2" t="inlineStr">
+        <is>
+          <t>720p</t>
+        </is>
+      </c>
+      <c r="AU2" t="inlineStr">
+        <is>
+          <t>Stereo</t>
+        </is>
+      </c>
+      <c r="AV2" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="AS3" t="inlineStr">
+      <c r="AW2" t="inlineStr">
+        <is>
+          <t>Built In Microphone</t>
+        </is>
+      </c>
+      <c r="AX2" t="inlineStr">
+        <is>
+          <t>Multi-Gesture Touchpad</t>
+        </is>
+      </c>
+      <c r="AY2" t="inlineStr">
+        <is>
+          <t>95Key Acer Keyboard Layout With International Language Support Including Indicators of CapsLock and F3/Microphone Mute</t>
+        </is>
+      </c>
+      <c r="AZ2" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="AT3" t="inlineStr">
-        <is>
-          <t>Wi-Fi 5</t>
-        </is>
-      </c>
-      <c r="AU3" t="inlineStr">
-        <is>
-          <t>v5.0</t>
-        </is>
-      </c>
-      <c r="AV3" t="inlineStr"/>
-      <c r="AW3" t="inlineStr">
-        <is>
-          <t>357.4 x 228 x 17.7 mm</t>
-        </is>
-      </c>
-      <c r="AX3" t="inlineStr">
-        <is>
-          <t>1.3 Kg</t>
-        </is>
-      </c>
-      <c r="AY3" t="inlineStr">
-        <is>
-          <t>Not Available</t>
-        </is>
-      </c>
-      <c r="AZ3" t="inlineStr">
-        <is>
-          <t>T-Type HD camera, Compatible with Windows only</t>
-        </is>
-      </c>
-      <c r="BA3" t="inlineStr"/>
-      <c r="BB3" t="inlineStr">
-        <is>
-          <t>84key Acer keyboard layout with international language support including indicators of CapsLock and F2/Microphone mute</t>
-        </is>
-      </c>
-      <c r="BC3" t="inlineStr"/>
-      <c r="BD3" t="inlineStr"/>
-      <c r="BE3" t="inlineStr">
-        <is>
-          <t>1 Year Carry-in Warranty</t>
-        </is>
-      </c>
-      <c r="BF3" t="inlineStr">
-        <is>
-          <t>Carry-in</t>
-        </is>
-      </c>
-      <c r="BG3" t="inlineStr">
-        <is>
-          <t>Manufacturing Defects</t>
-        </is>
-      </c>
-      <c r="BH3" t="inlineStr">
-        <is>
-          <t>Physical Damage</t>
-        </is>
-      </c>
-      <c r="BI3" t="inlineStr"/>
-      <c r="BJ3" t="inlineStr">
-        <is>
-          <t>1 x HDMI Port</t>
-        </is>
-      </c>
-      <c r="BK3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Acer Aspire 3 Intel Celeron Dual Core N4500 - (8 GB/512 GB SSD/Windows 11 Home) A325-45 Thin and Light Laptop  (15.6 Inch, Steel Grey, 1.50 Kg)</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>₹22,530</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>₹29,990</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Acer Aspire 3 Intel Celeron Dual Core N4500 - (8 GB/512 GB SSD/Windows 11 Home) A325-45 Thin and Light Laptop Rs.29990  Price in India - Buy Acer Aspire 3 Intel Celeron Dual Core N4500 - (8 GB/512 GB SSD/Windows 11 Home) A325-45 Thin and Light Laptop Steel Grey Online - Acer : Flipkart.com</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Acer Aspire 3 Intel Celeron Dual Core N4500 - (8 GB/512 GB SSD/Windows 11 Home) A325-45 Thin and Light Laptop Price, Acer Aspire 3 Intel Celeron Dual Core N4500 - (8 GB/512 GB SSD/Windows 11 Home) A325-45 Thin and Light Laptop Specifications, Acer Aspire 3 Intel Celeron Dual Core N4500 - (8 GB/512 GB SSD/Windows 11 Home) A325-45 Thin and Light Laptop Features</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Buy Acer Aspire 3 Intel Celeron Dual Core N4500 - (8 GB/512 GB SSD/Windows 11 Home) A325-45 Thin and Light Laptop Online For Rs.29990 , Also get Acer Aspire 3 Intel Celeron Dual Core N4500 - (8 GB/512 GB SSD/Windows 11 Home) A325-45 Thin and Light Laptop Specifications &amp; Features. Only Genuine Products. 30 Day Replacement Guarantee. Free Shipping. Cash On Delivery!</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>['https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/t/r/0/-original-imah3yhqbhu6fts2.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/d/6/p/-original-imah3yhqcgjtxfhw.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/d/b/q/-original-imah3yhqr4thfs9n.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/f/4/l/-original-imah3yhqhxrap3rd.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/w/e/r/-original-imah3yhqdhne9khd.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/w/c/4/-original-imah3yhqxzxzp5st.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/c/o/2/-original-imah3yhquwntysf7.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/a/u/u/-original-imah3yhqkjzh2xxe.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/5/l/y/-original-imah3yhqpzpfsjnm.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/s/2/a/-original-imah3yhqbgkhqqhm.jpeg?q=100&amp;crop=false']</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>Laptop, Power Adaptor, User Guide, Warranty Documents</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>A325-45</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>UN.344SI.004</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>A325-45</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>Aspire 3</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>Steel Grey</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>Thin and Light Laptop</t>
-        </is>
-      </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>Processing &amp; Multitasking</t>
-        </is>
-      </c>
-      <c r="Q4" t="inlineStr"/>
-      <c r="R4" t="inlineStr"/>
-      <c r="S4" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="T4" t="inlineStr">
-        <is>
-          <t>Intel</t>
-        </is>
-      </c>
-      <c r="U4" t="inlineStr">
-        <is>
-          <t>Celeron Dual Core</t>
-        </is>
-      </c>
-      <c r="V4" t="inlineStr">
+      <c r="BA2" t="inlineStr">
+        <is>
+          <t>1 Year</t>
+        </is>
+      </c>
+      <c r="BB2" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="W4" t="inlineStr">
-        <is>
-          <t>512 GB</t>
-        </is>
-      </c>
-      <c r="X4" t="inlineStr">
-        <is>
-          <t>8 GB</t>
-        </is>
-      </c>
-      <c r="Y4" t="inlineStr">
-        <is>
-          <t>LPDDR4X</t>
-        </is>
-      </c>
-      <c r="Z4" t="inlineStr">
-        <is>
-          <t>N4500</t>
-        </is>
-      </c>
-      <c r="AA4" t="inlineStr">
-        <is>
-          <t>Max Frequency upto 2.8 GHz</t>
-        </is>
-      </c>
-      <c r="AB4" t="inlineStr"/>
-      <c r="AC4" t="inlineStr"/>
-      <c r="AD4" t="inlineStr">
-        <is>
-          <t>Intel Integrated UHD</t>
-        </is>
-      </c>
-      <c r="AE4" t="inlineStr"/>
-      <c r="AF4" t="inlineStr">
-        <is>
-          <t>SSD</t>
-        </is>
-      </c>
-      <c r="AG4" t="inlineStr"/>
-      <c r="AH4" t="inlineStr">
-        <is>
-          <t>Windows 11 Home</t>
-        </is>
-      </c>
-      <c r="AI4" t="inlineStr"/>
-      <c r="AJ4" t="inlineStr"/>
-      <c r="AK4" t="inlineStr"/>
-      <c r="AL4" t="inlineStr"/>
-      <c r="AM4" t="inlineStr">
-        <is>
-          <t>1 x USB 3.0 ports</t>
-        </is>
-      </c>
-      <c r="AN4" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="AO4" t="inlineStr">
-        <is>
-          <t>39.62 cm (15.6 Inch)</t>
-        </is>
-      </c>
-      <c r="AP4" t="inlineStr">
-        <is>
-          <t>1366 x 768 Pixel</t>
-        </is>
-      </c>
-      <c r="AQ4" t="inlineStr">
-        <is>
-          <t>HD</t>
-        </is>
-      </c>
-      <c r="AR4" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="AS4" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="AT4" t="inlineStr">
-        <is>
-          <t>Wi-Fi 5</t>
-        </is>
-      </c>
-      <c r="AU4" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="AV4" t="inlineStr"/>
-      <c r="AW4" t="inlineStr">
-        <is>
-          <t>357.4 x 228 x 17.7 mm</t>
-        </is>
-      </c>
-      <c r="AX4" t="inlineStr">
-        <is>
-          <t>1.50 Kg</t>
-        </is>
-      </c>
-      <c r="AY4" t="inlineStr">
-        <is>
-          <t>Not Available</t>
-        </is>
-      </c>
-      <c r="AZ4" t="inlineStr">
-        <is>
-          <t>UFC with T-Type HD camera, Compatible with Windows only, 720p HD video at 30 fps with Temporal Noise Reduction, Blue Glass lens</t>
-        </is>
-      </c>
-      <c r="BA4" t="inlineStr"/>
-      <c r="BB4" t="inlineStr">
-        <is>
-          <t>95key Acer keyboard layout with international language support including indicators of CapsLock and F3/Microphone mute</t>
-        </is>
-      </c>
-      <c r="BC4" t="inlineStr"/>
-      <c r="BD4" t="inlineStr"/>
-      <c r="BE4" t="inlineStr">
-        <is>
-          <t>1 Year Onsite Warranty</t>
-        </is>
-      </c>
-      <c r="BF4" t="inlineStr">
-        <is>
-          <t>Onsite</t>
-        </is>
-      </c>
-      <c r="BG4" t="inlineStr">
-        <is>
-          <t>Manufacturing Defects</t>
-        </is>
-      </c>
-      <c r="BH4" t="inlineStr">
-        <is>
-          <t>Physical Damage</t>
-        </is>
-      </c>
-      <c r="BI4" t="inlineStr"/>
-      <c r="BJ4" t="inlineStr"/>
-      <c r="BK4" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Acer Aspire 3 Spin 14 Intel Core i3 13th Gen N305 - (8 GB/512 GB SSD/Windows 11 Home) A3SP14-31PT-3554 Thin and Light Laptop  (14 inch, Silver, 1.54 Kg, With MS Office)</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>₹40,100</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>₹55,140</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>In the world of laptops, where innovation meets functionality, the Acer Aspire 3 Spin 14 emerges as a versatile virtuoso, transcending the boundaries of conventional computing. With a design that seamlessly blends thinness, lightness, and versatility, this 2-in-1 convertible laptop is not just a device; it's a gateway to a world where your ideas come to life. It's not just a laptop; it's an experience that unfolds with every flip, every touch, and every task. As you delve into the thin, light, and versatile world of this convertible laptop, you realize it's not just a device; it's a companion that enhances your journey through the digital realm. Welcome to a new era of computing; welcome to the Acer Aspire 3 Spin 14 experience.</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Acer Aspire 3 Spin 14 Intel Core i3 13th Gen N305 - (8 GB/512 GB SSD/Windows 11 Home) A3SP14-31PT-3554 Thin and Light Laptop Rs.55140  Price in India - Buy Acer Aspire 3 Spin 14 Intel Core i3 13th Gen N305 - (8 GB/512 GB SSD/Windows 11 Home) A3SP14-31PT-3554 Thin and Light Laptop Silver Online - Acer : Flipkart.com</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Acer Aspire 3 Spin 14 Intel Core i3 13th Gen N305 - (8 GB/512 GB SSD/Windows 11 Home) A3SP14-31PT-3554 Thin and Light Laptop Price, Acer Aspire 3 Spin 14 Intel Core i3 13th Gen N305 - (8 GB/512 GB SSD/Windows 11 Home) A3SP14-31PT-3554 Thin and Light Laptop Specifications, Acer Aspire 3 Spin 14 Intel Core i3 13th Gen N305 - (8 GB/512 GB SSD/Windows 11 Home) A3SP14-31PT-3554 Thin and Light Laptop Features</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Buy Acer Aspire 3 Spin 14 Intel Core i3 13th Gen N305 - (8 GB/512 GB SSD/Windows 11 Home) A3SP14-31PT-3554 Thin and Light Laptop Online For Rs.55140 , Also get Acer Aspire 3 Spin 14 Intel Core i3 13th Gen N305 - (8 GB/512 GB SSD/Windows 11 Home) A3SP14-31PT-3554 Thin and Light Laptop Specifications &amp; Features. Only Genuine Products. 30 Day Replacement Guarantee. Free Shipping. Cash On Delivery!</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>['https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/q/j/a/a3sp14-31pt-thin-and-light-laptop-acer-original-imah4bj3nvfzgk9g.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/f/w/y/a3sp14-31pt-thin-and-light-laptop-acer-original-imah4bj3ggcejgxd.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/i/n/p/a3sp14-31pt-thin-and-light-laptop-acer-original-imah4bj3jtt5ht8g.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/i/2/e/a3sp14-31pt-thin-and-light-laptop-acer-original-imah4bj3zty7uwzt.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/p/j/o/a3sp14-31pt-thin-and-light-laptop-acer-original-imah4bj3vxnbzuzx.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/z/m/n/a3sp14-31pt-thin-and-light-laptop-acer-original-imah4bj3v9f9uqff.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/x/u/3/a3sp14-31pt-thin-and-light-laptop-acer-original-imah4bj3kzhphypa.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/d/p/j/-original-imagwkaymfh66hw3.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/g/f/r/a3sp14-31pt-thin-and-light-laptop-acer-original-imah4bj3b5edadhw.jpeg?q=100&amp;crop=false']</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>Laptop, Power Adaptor, User Guide, Warranty Documents</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>A3SP14-31PT-3554</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>NX.KENSI.004</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>A3SP14-31PT</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>Aspire 3 Spin 14</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>Silver</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>Thin and Light Laptop</t>
-        </is>
-      </c>
-      <c r="P5" t="inlineStr">
-        <is>
-          <t>Processing &amp; Multitasking</t>
-        </is>
-      </c>
-      <c r="Q5" t="inlineStr"/>
-      <c r="R5" t="inlineStr"/>
-      <c r="S5" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="T5" t="inlineStr">
-        <is>
-          <t>Intel</t>
-        </is>
-      </c>
-      <c r="U5" t="inlineStr">
-        <is>
-          <t>Core i3</t>
-        </is>
-      </c>
-      <c r="V5" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="W5" t="inlineStr">
-        <is>
-          <t>512 GB</t>
-        </is>
-      </c>
-      <c r="X5" t="inlineStr">
-        <is>
-          <t>8 GB</t>
-        </is>
-      </c>
-      <c r="Y5" t="inlineStr">
-        <is>
-          <t>LPDDR5</t>
-        </is>
-      </c>
-      <c r="Z5" t="inlineStr">
-        <is>
-          <t>N305</t>
-        </is>
-      </c>
-      <c r="AA5" t="inlineStr">
-        <is>
-          <t>Max Frequency Up to 3.8 GHz</t>
-        </is>
-      </c>
-      <c r="AB5" t="inlineStr"/>
-      <c r="AC5" t="inlineStr"/>
-      <c r="AD5" t="inlineStr">
-        <is>
-          <t>Intel Integrated UHD</t>
-        </is>
-      </c>
-      <c r="AE5" t="inlineStr"/>
-      <c r="AF5" t="inlineStr">
-        <is>
-          <t>SSD</t>
-        </is>
-      </c>
-      <c r="AG5" t="inlineStr"/>
-      <c r="AH5" t="inlineStr">
-        <is>
-          <t>Windows 11 Home</t>
-        </is>
-      </c>
-      <c r="AI5" t="inlineStr"/>
-      <c r="AJ5" t="inlineStr"/>
-      <c r="AK5" t="inlineStr"/>
-      <c r="AL5" t="inlineStr"/>
-      <c r="AM5" t="inlineStr">
-        <is>
-          <t>1 x USB Type-C port with DC-in, 2 x USB 3.2 port</t>
-        </is>
-      </c>
-      <c r="AN5" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="AO5" t="inlineStr">
-        <is>
-          <t>35.56 cm (14 inch)</t>
-        </is>
-      </c>
-      <c r="AP5" t="inlineStr">
-        <is>
-          <t>1920 x 1200 Pixel</t>
-        </is>
-      </c>
-      <c r="AQ5" t="inlineStr">
-        <is>
-          <t>Full HD, TFT, LCD</t>
-        </is>
-      </c>
-      <c r="AR5" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="AS5" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="AT5" t="inlineStr">
-        <is>
-          <t>WIFI6+BT - 1x1 AX</t>
-        </is>
-      </c>
-      <c r="AU5" t="inlineStr">
-        <is>
-          <t>v5.2</t>
-        </is>
-      </c>
-      <c r="AV5" t="inlineStr"/>
-      <c r="AW5" t="inlineStr">
-        <is>
-          <t>319.8 x 227.9 x 18.9 mm</t>
-        </is>
-      </c>
-      <c r="AX5" t="inlineStr">
-        <is>
-          <t>1.54 Kg</t>
-        </is>
-      </c>
-      <c r="AY5" t="inlineStr">
-        <is>
-          <t>Not Available</t>
-        </is>
-      </c>
-      <c r="AZ5" t="inlineStr">
-        <is>
-          <t>T-Type HD camera with 1280 x 720 resolution and 720p HD video at 30 fps with Temporal Noise Reduction</t>
-        </is>
-      </c>
-      <c r="BA5" t="inlineStr"/>
-      <c r="BB5" t="inlineStr">
-        <is>
-          <t>80-/81-/84-key Acer keyboard layout with international language support including indicators of CapsLock and F4/Microphone mute</t>
-        </is>
-      </c>
-      <c r="BC5" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="BD5" t="inlineStr"/>
-      <c r="BE5" t="inlineStr">
-        <is>
-          <t>1 Year Onsite Warranty</t>
-        </is>
-      </c>
-      <c r="BF5" t="inlineStr">
-        <is>
-          <t>Onsite</t>
-        </is>
-      </c>
-      <c r="BG5" t="inlineStr">
-        <is>
-          <t>Manufacturing Defects</t>
-        </is>
-      </c>
-      <c r="BH5" t="inlineStr">
-        <is>
-          <t>Physical Damage</t>
-        </is>
-      </c>
-      <c r="BI5" t="inlineStr"/>
-      <c r="BJ5" t="inlineStr"/>
-      <c r="BK5" t="inlineStr">
-        <is>
-          <t>13th Gen</t>
+      <c r="BC2" t="inlineStr">
+        <is>
+          <t>Laptop, Power Adapter, User Manual, Warranty Card</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: Extract unique product IDs from Flipkart and Amazon URLs
- Added logic to extract unique IDs:
  - Flipkart: Extracts the 12-character unique ID after 'itm' in the URL.
  - Amazon: Extracts the 10-character unique ID after 'dp/' in the URL.

- Ensured robustness:
  - Validates and trims IDs to the appropriate length.
  - Defaults to 'NA' if no valid ID is found.
  - Added error handling with logging for failures.

- Improved modularity:
  - Reusable logic to handle URL splitting and segment matching for both platforms.
</commit_message>
<xml_diff>
--- a/data/output_scraper_results.xlsx
+++ b/data/output_scraper_results.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BJ3"/>
+  <dimension ref="A1:BK3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,275 +473,280 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
+          <t>Unique</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
           <t>Images</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Sales Package</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Model Number</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Part Number</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Model Name</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Series</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Color</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Type</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Suitable For</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>Power Supply</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>Battery Cell</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>MS Office Provided</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>Processor Brand</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>Processor Name</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>SSD</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>SSD Capacity</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>RAM</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>RAM Type</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>Processor Variant</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>Clock Speed</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>Memory Slots</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>Expandable Memory</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>Graphic Processor</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>Number of Cores</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>Storage Type</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>OS Architecture</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>Operating System</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>Supported Operating System</t>
         </is>
       </c>
-      <c r="AJ1" s="1" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>System Architecture</t>
         </is>
       </c>
-      <c r="AK1" s="1" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>Mic In</t>
         </is>
       </c>
-      <c r="AL1" s="1" t="inlineStr">
+      <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>RJ45</t>
         </is>
       </c>
-      <c r="AM1" s="1" t="inlineStr">
+      <c r="AN1" s="1" t="inlineStr">
         <is>
           <t>USB Port</t>
         </is>
       </c>
-      <c r="AN1" s="1" t="inlineStr">
+      <c r="AO1" s="1" t="inlineStr">
         <is>
           <t>Touchscreen</t>
         </is>
       </c>
-      <c r="AO1" s="1" t="inlineStr">
+      <c r="AP1" s="1" t="inlineStr">
         <is>
           <t>Screen Size</t>
         </is>
       </c>
-      <c r="AP1" s="1" t="inlineStr">
+      <c r="AQ1" s="1" t="inlineStr">
         <is>
           <t>Screen Resolution</t>
         </is>
       </c>
-      <c r="AQ1" s="1" t="inlineStr">
+      <c r="AR1" s="1" t="inlineStr">
         <is>
           <t>Screen Type</t>
         </is>
       </c>
-      <c r="AR1" s="1" t="inlineStr">
+      <c r="AS1" s="1" t="inlineStr">
         <is>
           <t>Speakers</t>
         </is>
       </c>
-      <c r="AS1" s="1" t="inlineStr">
+      <c r="AT1" s="1" t="inlineStr">
         <is>
           <t>Internal Mic</t>
         </is>
       </c>
-      <c r="AT1" s="1" t="inlineStr">
+      <c r="AU1" s="1" t="inlineStr">
         <is>
           <t>Wireless LAN</t>
         </is>
       </c>
-      <c r="AU1" s="1" t="inlineStr">
+      <c r="AV1" s="1" t="inlineStr">
         <is>
           <t>Bluetooth</t>
         </is>
       </c>
-      <c r="AV1" s="1" t="inlineStr">
+      <c r="AW1" s="1" t="inlineStr">
         <is>
           <t>Ethernet</t>
         </is>
       </c>
-      <c r="AW1" s="1" t="inlineStr">
+      <c r="AX1" s="1" t="inlineStr">
         <is>
           <t>Dimensions</t>
         </is>
       </c>
-      <c r="AX1" s="1" t="inlineStr">
+      <c r="AY1" s="1" t="inlineStr">
         <is>
           <t>Weight</t>
         </is>
       </c>
-      <c r="AY1" s="1" t="inlineStr">
+      <c r="AZ1" s="1" t="inlineStr">
         <is>
           <t>Disk Drive</t>
         </is>
       </c>
-      <c r="AZ1" s="1" t="inlineStr">
+      <c r="BA1" s="1" t="inlineStr">
         <is>
           <t>Web Camera</t>
         </is>
       </c>
-      <c r="BA1" s="1" t="inlineStr">
+      <c r="BB1" s="1" t="inlineStr">
         <is>
           <t>Lock Port</t>
         </is>
       </c>
-      <c r="BB1" s="1" t="inlineStr">
+      <c r="BC1" s="1" t="inlineStr">
         <is>
           <t>Keyboard</t>
         </is>
       </c>
-      <c r="BC1" s="1" t="inlineStr">
+      <c r="BD1" s="1" t="inlineStr">
         <is>
           <t>Backlit Keyboard</t>
         </is>
       </c>
-      <c r="BD1" s="1" t="inlineStr">
+      <c r="BE1" s="1" t="inlineStr">
         <is>
           <t>Pointer Device</t>
         </is>
       </c>
-      <c r="BE1" s="1" t="inlineStr">
+      <c r="BF1" s="1" t="inlineStr">
         <is>
           <t>Warranty Summary</t>
         </is>
       </c>
-      <c r="BF1" s="1" t="inlineStr">
+      <c r="BG1" s="1" t="inlineStr">
         <is>
           <t>Warranty Service Type</t>
         </is>
       </c>
-      <c r="BG1" s="1" t="inlineStr">
+      <c r="BH1" s="1" t="inlineStr">
         <is>
           <t>Covered in Warranty</t>
         </is>
       </c>
-      <c r="BH1" s="1" t="inlineStr">
+      <c r="BI1" s="1" t="inlineStr">
         <is>
           <t>Not Covered in Warranty</t>
         </is>
       </c>
-      <c r="BI1" s="1" t="inlineStr">
+      <c r="BJ1" s="1" t="inlineStr">
         <is>
           <t>International Warranty</t>
         </is>
       </c>
-      <c r="BJ1" s="1" t="inlineStr">
+      <c r="BK1" s="1" t="inlineStr">
         <is>
           <t>Processor Generation</t>
         </is>
@@ -785,260 +790,265 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>['https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/v/t/b/-original-imagvkpfbpgzzqfe.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/3/j/a/z2-493-thin-and-light-laptop-acer-original-imagr6yjpmhhmpvm.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/o/x/n/-original-imagzk3kuu8kduxk.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/x/h/l/-original-imagzk3kcpg6fzxf.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/d/u/y/-original-imagzk3kukhhjdhq.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/l/u/v/z2-493-thin-and-light-laptop-acer-original-imagr6yjuvhjntcb.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/a/i/i/-original-imagzk3kfk6bktha.jpeg?q=100&amp;crop=false']</t>
+          <t>752c735b4b0a</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
+          <t>['https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/x/h/l/-original-imagzk3kcpg6fzxf.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/o/x/n/-original-imagzk3kuu8kduxk.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/d/u/y/-original-imagzk3kukhhjdhq.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/3/j/a/z2-493-thin-and-light-laptop-acer-original-imagr6yjpmhhmpvm.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/l/u/v/z2-493-thin-and-light-laptop-acer-original-imagr6yjuvhjntcb.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/v/t/b/-original-imagvkpfbpgzzqfe.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/a/i/i/-original-imagzk3kfk6bktha.jpeg?q=100&amp;crop=false']</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
           <t>Laptop, Power Adaptor, User Guide, Warranty Documents</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="K2" t="inlineStr">
         <is>
           <t>Z2-493</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="L2" t="inlineStr">
         <is>
           <t>UN.31USI.006|UN.431SI.146</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
+      <c r="M2" t="inlineStr">
         <is>
           <t>Z2-493</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
+      <c r="N2" t="inlineStr">
         <is>
           <t>One 14</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
+      <c r="O2" t="inlineStr">
         <is>
           <t>Silver</t>
         </is>
       </c>
-      <c r="O2" t="inlineStr">
+      <c r="P2" t="inlineStr">
         <is>
           <t>Thin and Light Laptop</t>
         </is>
       </c>
-      <c r="P2" t="inlineStr">
+      <c r="Q2" t="inlineStr">
         <is>
           <t>Everyday Use, Processing &amp; Multitasking, Travel &amp; Business</t>
         </is>
       </c>
-      <c r="Q2" t="inlineStr">
+      <c r="R2" t="inlineStr">
         <is>
           <t>50 Hz AC power adapter</t>
         </is>
       </c>
-      <c r="R2" t="n">
+      <c r="S2" t="n">
         <v>3</v>
       </c>
-      <c r="S2" t="inlineStr">
+      <c r="T2" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="T2" t="inlineStr">
+      <c r="U2" t="inlineStr">
         <is>
           <t>AMD</t>
         </is>
       </c>
-      <c r="U2" t="inlineStr">
+      <c r="V2" t="inlineStr">
         <is>
           <t>Ryzen 3 Dual Core</t>
         </is>
       </c>
-      <c r="V2" t="inlineStr">
+      <c r="W2" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="W2" t="inlineStr">
+      <c r="X2" t="inlineStr">
         <is>
           <t>256 GB</t>
         </is>
       </c>
-      <c r="X2" t="inlineStr">
+      <c r="Y2" t="inlineStr">
         <is>
           <t>8 GB</t>
         </is>
       </c>
-      <c r="Y2" t="inlineStr">
+      <c r="Z2" t="inlineStr">
         <is>
           <t>DDR4</t>
         </is>
       </c>
-      <c r="Z2" t="inlineStr">
+      <c r="AA2" t="inlineStr">
         <is>
           <t>3250U</t>
         </is>
       </c>
-      <c r="AA2" t="inlineStr">
+      <c r="AB2" t="inlineStr">
         <is>
           <t>2.60 Ghz with Max Turbo Frequency up to 3.5 Ghz</t>
         </is>
       </c>
-      <c r="AB2" t="n">
+      <c r="AC2" t="n">
         <v>2</v>
       </c>
-      <c r="AC2" t="n">
+      <c r="AD2" t="n">
         <v>32</v>
       </c>
-      <c r="AD2" t="inlineStr">
+      <c r="AE2" t="inlineStr">
         <is>
           <t>AMD Radeon Radeon Graphics</t>
         </is>
       </c>
-      <c r="AE2" t="n">
+      <c r="AF2" t="n">
         <v>2</v>
       </c>
-      <c r="AF2" t="inlineStr">
+      <c r="AG2" t="inlineStr">
         <is>
           <t>SSD</t>
         </is>
       </c>
-      <c r="AG2" t="inlineStr">
+      <c r="AH2" t="inlineStr">
         <is>
           <t>64 bit</t>
         </is>
       </c>
-      <c r="AH2" t="inlineStr">
+      <c r="AI2" t="inlineStr">
         <is>
           <t>Windows 11 Home</t>
         </is>
       </c>
-      <c r="AI2" t="inlineStr">
+      <c r="AJ2" t="inlineStr">
         <is>
           <t>Windows 11 Home</t>
         </is>
       </c>
-      <c r="AJ2" t="n">
+      <c r="AK2" t="n">
         <v>64</v>
       </c>
-      <c r="AK2" t="inlineStr">
+      <c r="AL2" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="AL2" t="inlineStr">
+      <c r="AM2" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="AM2" t="inlineStr">
+      <c r="AN2" t="inlineStr">
         <is>
           <t>2 x USB 3.2 Gen 1 Type, 1 x USB 3.2 (Gen1) Type C</t>
         </is>
       </c>
-      <c r="AN2" t="inlineStr">
+      <c r="AO2" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="AO2" t="inlineStr">
+      <c r="AP2" t="inlineStr">
         <is>
           <t>35.56 cm (14 inch)</t>
         </is>
       </c>
-      <c r="AP2" t="inlineStr">
+      <c r="AQ2" t="inlineStr">
         <is>
           <t>1366 x 768 Pixels</t>
         </is>
       </c>
-      <c r="AQ2" t="inlineStr">
+      <c r="AR2" t="inlineStr">
         <is>
           <t>HD, Acer ComfyView LED-backlit TFT LCD</t>
         </is>
       </c>
-      <c r="AR2" t="inlineStr">
+      <c r="AS2" t="inlineStr">
         <is>
           <t>Two built-in speakers</t>
         </is>
       </c>
-      <c r="AS2" t="inlineStr">
+      <c r="AT2" t="inlineStr">
         <is>
           <t>Built-in Dual Microphones</t>
         </is>
       </c>
-      <c r="AT2" t="inlineStr">
+      <c r="AU2" t="inlineStr">
         <is>
           <t>802.11b/g/n/ac wireless LAN</t>
         </is>
       </c>
-      <c r="AU2" t="inlineStr">
+      <c r="AV2" t="inlineStr">
         <is>
           <t>v4.2</t>
         </is>
       </c>
-      <c r="AV2" t="inlineStr">
+      <c r="AW2" t="inlineStr">
         <is>
           <t>Gigabit Ethernet</t>
         </is>
       </c>
-      <c r="AW2" t="inlineStr">
+      <c r="AX2" t="inlineStr">
         <is>
           <t>325.9 x 226.9 x 20.9 mm</t>
         </is>
       </c>
-      <c r="AX2" t="inlineStr">
+      <c r="AY2" t="inlineStr">
         <is>
           <t>1.5 Kg</t>
         </is>
       </c>
-      <c r="AY2" t="inlineStr">
+      <c r="AZ2" t="inlineStr">
         <is>
           <t>Not Available</t>
         </is>
       </c>
-      <c r="AZ2" t="inlineStr">
+      <c r="BA2" t="inlineStr">
         <is>
           <t>HD Webcam</t>
         </is>
       </c>
-      <c r="BA2" t="inlineStr">
+      <c r="BB2" t="inlineStr">
         <is>
           <t>Security Lock Slot</t>
         </is>
       </c>
-      <c r="BB2" t="inlineStr">
+      <c r="BC2" t="inlineStr">
         <is>
           <t>Isolated Keys keyboard with touchpad with multi gesture and scrolling Function</t>
         </is>
       </c>
-      <c r="BC2" t="inlineStr">
+      <c r="BD2" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="BD2" t="inlineStr">
+      <c r="BE2" t="inlineStr">
         <is>
           <t>Touchpad with Multi-touch Gesture Support</t>
         </is>
       </c>
-      <c r="BE2" t="inlineStr">
+      <c r="BF2" t="inlineStr">
         <is>
           <t>1 Year International Travelers Warranty (ITW)</t>
         </is>
       </c>
-      <c r="BF2" t="inlineStr">
+      <c r="BG2" t="inlineStr">
         <is>
           <t>Onsite</t>
         </is>
       </c>
-      <c r="BG2" t="inlineStr">
+      <c r="BH2" t="inlineStr">
         <is>
           <t>Manufacturing Defects</t>
         </is>
       </c>
-      <c r="BH2" t="inlineStr">
+      <c r="BI2" t="inlineStr">
         <is>
           <t>Physical Damage</t>
         </is>
       </c>
-      <c r="BI2" t="inlineStr">
+      <c r="BJ2" t="inlineStr">
         <is>
           <t>1 Year</t>
         </is>
@@ -1082,205 +1092,210 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>['https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/i/2/e/a3sp14-31pt-thin-and-light-laptop-acer-original-imah4bj3zty7uwzt.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/i/n/p/a3sp14-31pt-thin-and-light-laptop-acer-original-imah4bj3jtt5ht8g.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/g/f/r/a3sp14-31pt-thin-and-light-laptop-acer-original-imah4bj3b5edadhw.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/d/p/j/-original-imagwkaymfh66hw3.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/p/j/o/a3sp14-31pt-thin-and-light-laptop-acer-original-imah4bj3vxnbzuzx.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/f/w/y/a3sp14-31pt-thin-and-light-laptop-acer-original-imah4bj3ggcejgxd.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/z/m/n/a3sp14-31pt-thin-and-light-laptop-acer-original-imah4bj3v9f9uqff.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/x/u/3/a3sp14-31pt-thin-and-light-laptop-acer-original-imah4bj3kzhphypa.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/q/j/a/a3sp14-31pt-thin-and-light-laptop-acer-original-imah4bj3nvfzgk9g.jpeg?q=100&amp;crop=false']</t>
+          <t>3adc9b4b7ed0</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
+          <t>['https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/f/w/y/a3sp14-31pt-thin-and-light-laptop-acer-original-imah4bj3ggcejgxd.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/i/n/p/a3sp14-31pt-thin-and-light-laptop-acer-original-imah4bj3jtt5ht8g.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/p/j/o/a3sp14-31pt-thin-and-light-laptop-acer-original-imah4bj3vxnbzuzx.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/g/f/r/a3sp14-31pt-thin-and-light-laptop-acer-original-imah4bj3b5edadhw.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/x/u/3/a3sp14-31pt-thin-and-light-laptop-acer-original-imah4bj3kzhphypa.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/z/m/n/a3sp14-31pt-thin-and-light-laptop-acer-original-imah4bj3v9f9uqff.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/i/2/e/a3sp14-31pt-thin-and-light-laptop-acer-original-imah4bj3zty7uwzt.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/q/j/a/a3sp14-31pt-thin-and-light-laptop-acer-original-imah4bj3nvfzgk9g.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/d/p/j/-original-imagwkaymfh66hw3.jpeg?q=100&amp;crop=false']</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
           <t>Laptop, Power Adaptor, User Guide, Warranty Documents</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="K3" t="inlineStr">
         <is>
           <t>A3SP14-31PT-3554</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr">
+      <c r="L3" t="inlineStr">
         <is>
           <t>NX.KENSI.004</t>
         </is>
       </c>
-      <c r="L3" t="inlineStr">
+      <c r="M3" t="inlineStr">
         <is>
           <t>A3SP14-31PT</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr">
+      <c r="N3" t="inlineStr">
         <is>
           <t>Aspire 3 Spin 14</t>
         </is>
       </c>
-      <c r="N3" t="inlineStr">
+      <c r="O3" t="inlineStr">
         <is>
           <t>Silver</t>
         </is>
       </c>
-      <c r="O3" t="inlineStr">
+      <c r="P3" t="inlineStr">
         <is>
           <t>Thin and Light Laptop</t>
         </is>
       </c>
-      <c r="P3" t="inlineStr">
+      <c r="Q3" t="inlineStr">
         <is>
           <t>Processing &amp; Multitasking</t>
         </is>
       </c>
-      <c r="S3" t="inlineStr">
+      <c r="T3" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="T3" t="inlineStr">
+      <c r="U3" t="inlineStr">
         <is>
           <t>Intel</t>
         </is>
       </c>
-      <c r="U3" t="inlineStr">
+      <c r="V3" t="inlineStr">
         <is>
           <t>Core i3</t>
         </is>
       </c>
-      <c r="V3" t="inlineStr">
+      <c r="W3" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="W3" t="inlineStr">
+      <c r="X3" t="inlineStr">
         <is>
           <t>512 GB</t>
         </is>
       </c>
-      <c r="X3" t="inlineStr">
+      <c r="Y3" t="inlineStr">
         <is>
           <t>8 GB</t>
         </is>
       </c>
-      <c r="Y3" t="inlineStr">
+      <c r="Z3" t="inlineStr">
         <is>
           <t>LPDDR5</t>
         </is>
       </c>
-      <c r="Z3" t="inlineStr">
+      <c r="AA3" t="inlineStr">
         <is>
           <t>N305</t>
         </is>
       </c>
-      <c r="AA3" t="inlineStr">
+      <c r="AB3" t="inlineStr">
         <is>
           <t>Max Frequency Up to 3.8 GHz</t>
         </is>
       </c>
-      <c r="AD3" t="inlineStr">
+      <c r="AE3" t="inlineStr">
         <is>
           <t>Intel Integrated UHD</t>
         </is>
       </c>
-      <c r="AF3" t="inlineStr">
+      <c r="AG3" t="inlineStr">
         <is>
           <t>SSD</t>
         </is>
       </c>
-      <c r="AH3" t="inlineStr">
+      <c r="AI3" t="inlineStr">
         <is>
           <t>Windows 11 Home</t>
         </is>
       </c>
-      <c r="AM3" t="inlineStr">
+      <c r="AN3" t="inlineStr">
         <is>
           <t>1 x USB Type-C port with DC-in, 2 x USB 3.2 port</t>
         </is>
       </c>
-      <c r="AN3" t="inlineStr">
+      <c r="AO3" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="AO3" t="inlineStr">
+      <c r="AP3" t="inlineStr">
         <is>
           <t>35.56 cm (14 inch)</t>
         </is>
       </c>
-      <c r="AP3" t="inlineStr">
+      <c r="AQ3" t="inlineStr">
         <is>
           <t>1920 x 1200 Pixel</t>
         </is>
       </c>
-      <c r="AQ3" t="inlineStr">
+      <c r="AR3" t="inlineStr">
         <is>
           <t>Full HD, TFT, LCD</t>
         </is>
       </c>
-      <c r="AR3" t="inlineStr">
+      <c r="AS3" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="AS3" t="inlineStr">
+      <c r="AT3" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="AT3" t="inlineStr">
+      <c r="AU3" t="inlineStr">
         <is>
           <t>WIFI6+BT - 1x1 AX</t>
         </is>
       </c>
-      <c r="AU3" t="inlineStr">
+      <c r="AV3" t="inlineStr">
         <is>
           <t>v5.2</t>
         </is>
       </c>
-      <c r="AW3" t="inlineStr">
+      <c r="AX3" t="inlineStr">
         <is>
           <t>319.8 x 227.9 x 18.9 mm</t>
         </is>
       </c>
-      <c r="AX3" t="inlineStr">
+      <c r="AY3" t="inlineStr">
         <is>
           <t>1.54 Kg</t>
         </is>
       </c>
-      <c r="AY3" t="inlineStr">
+      <c r="AZ3" t="inlineStr">
         <is>
           <t>Not Available</t>
         </is>
       </c>
-      <c r="AZ3" t="inlineStr">
+      <c r="BA3" t="inlineStr">
         <is>
           <t>T-Type HD camera with 1280 x 720 resolution and 720p HD video at 30 fps with Temporal Noise Reduction</t>
         </is>
       </c>
-      <c r="BB3" t="inlineStr">
+      <c r="BC3" t="inlineStr">
         <is>
           <t>80-/81-/84-key Acer keyboard layout with international language support including indicators of CapsLock and F4/Microphone mute</t>
         </is>
       </c>
-      <c r="BC3" t="inlineStr">
+      <c r="BD3" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="BE3" t="inlineStr">
+      <c r="BF3" t="inlineStr">
         <is>
           <t>1 Year Onsite Warranty</t>
         </is>
       </c>
-      <c r="BF3" t="inlineStr">
+      <c r="BG3" t="inlineStr">
         <is>
           <t>Onsite</t>
         </is>
       </c>
-      <c r="BG3" t="inlineStr">
+      <c r="BH3" t="inlineStr">
         <is>
           <t>Manufacturing Defects</t>
         </is>
       </c>
-      <c r="BH3" t="inlineStr">
+      <c r="BI3" t="inlineStr">
         <is>
           <t>Physical Damage</t>
         </is>
       </c>
-      <c r="BJ3" t="inlineStr">
+      <c r="BK3" t="inlineStr">
         <is>
           <t>13th Gen</t>
         </is>
@@ -1375,7 +1390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BC2"/>
+  <dimension ref="A1:BG2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1406,255 +1421,275 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>Meta Title</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Meta Keywords</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Meta Description</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Unique</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
           <t>Images</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Name</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Brand</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Model</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Series</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Thickness</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Dimensions (WxDxH)</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Weight</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Colour(s)</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>Operating System</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>Operating System Type</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>Display Size</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>Display Resolution</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>Pixel Density</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>Display Features</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>Touchscreen</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>Aspect Ratio</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>Processor</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>Number of Cores</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>Graphic Processor</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>Capacity</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>RAM type</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>Memory Slots</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>Expandable Memory</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>Memory Layout</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>SSD Capacity</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>Battery Cell</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>Battery type</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>Power Supply</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>Battery Capacity</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>Wireless LAN</t>
         </is>
       </c>
-      <c r="AJ1" s="1" t="inlineStr">
+      <c r="AN1" s="1" t="inlineStr">
         <is>
           <t>Wi-Fi Version</t>
         </is>
       </c>
-      <c r="AK1" s="1" t="inlineStr">
+      <c r="AO1" s="1" t="inlineStr">
         <is>
           <t>Bluetooth</t>
         </is>
       </c>
-      <c r="AL1" s="1" t="inlineStr">
+      <c r="AP1" s="1" t="inlineStr">
         <is>
           <t>Bluetooth Version</t>
         </is>
       </c>
-      <c r="AM1" s="1" t="inlineStr">
+      <c r="AQ1" s="1" t="inlineStr">
         <is>
           <t>HDMI Ports</t>
         </is>
       </c>
-      <c r="AN1" s="1" t="inlineStr">
+      <c r="AR1" s="1" t="inlineStr">
         <is>
           <t>USB Type C</t>
         </is>
       </c>
-      <c r="AO1" s="1" t="inlineStr">
+      <c r="AS1" s="1" t="inlineStr">
         <is>
           <t>SD Card Reader</t>
         </is>
       </c>
-      <c r="AP1" s="1" t="inlineStr">
+      <c r="AT1" s="1" t="inlineStr">
         <is>
           <t>Headphone Jack</t>
         </is>
       </c>
-      <c r="AQ1" s="1" t="inlineStr">
+      <c r="AU1" s="1" t="inlineStr">
         <is>
           <t>Microphone Jack</t>
         </is>
       </c>
-      <c r="AR1" s="1" t="inlineStr">
+      <c r="AV1" s="1" t="inlineStr">
         <is>
           <t>VGA Port</t>
         </is>
       </c>
-      <c r="AS1" s="1" t="inlineStr">
+      <c r="AW1" s="1" t="inlineStr">
         <is>
           <t>Webcam</t>
         </is>
       </c>
-      <c r="AT1" s="1" t="inlineStr">
+      <c r="AX1" s="1" t="inlineStr">
         <is>
           <t>Video Recording</t>
         </is>
       </c>
-      <c r="AU1" s="1" t="inlineStr">
+      <c r="AY1" s="1" t="inlineStr">
         <is>
           <t>Speakers</t>
         </is>
       </c>
-      <c r="AV1" s="1" t="inlineStr">
+      <c r="AZ1" s="1" t="inlineStr">
         <is>
           <t>In-built Microphone</t>
         </is>
       </c>
-      <c r="AW1" s="1" t="inlineStr">
+      <c r="BA1" s="1" t="inlineStr">
         <is>
           <t>Microphone Type</t>
         </is>
       </c>
-      <c r="AX1" s="1" t="inlineStr">
+      <c r="BB1" s="1" t="inlineStr">
         <is>
           <t>Pointing Device</t>
         </is>
       </c>
-      <c r="AY1" s="1" t="inlineStr">
+      <c r="BC1" s="1" t="inlineStr">
         <is>
           <t>Keyboard</t>
         </is>
       </c>
-      <c r="AZ1" s="1" t="inlineStr">
+      <c r="BD1" s="1" t="inlineStr">
         <is>
           <t>Face Recognition</t>
         </is>
       </c>
-      <c r="BA1" s="1" t="inlineStr">
+      <c r="BE1" s="1" t="inlineStr">
         <is>
           <t>Warranty</t>
         </is>
       </c>
-      <c r="BB1" s="1" t="inlineStr">
+      <c r="BF1" s="1" t="inlineStr">
         <is>
           <t>Lockport</t>
         </is>
       </c>
-      <c r="BC1" s="1" t="inlineStr">
+      <c r="BG1" s="1" t="inlineStr">
         <is>
           <t>Sales Package</t>
         </is>
@@ -1683,75 +1718,95 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>['https://m.media-amazon.com/images/I/61qlqvTsocL._SL1664_.jpg', 'https://m.media-amazon.com/images/I/71Mwxs8TX+L._SL1664_.jpg', 'https://m.media-amazon.com/images/I/71p+Rn+JgbL._SL1664_.jpg', 'https://m.media-amazon.com/images/I/71W6EmfwI-L._SL1664_.jpg', 'https://m.media-amazon.com/images/I/71MllJzfDfL._SL1664_.jpg', 'https://m.media-amazon.com/images/I/71V25H7JYBL._SL1664_.jpg']</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>B0D7PYTTGH</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>['https://m.media-amazon.com/images/I/71p+Rn+JgbL._SL1664_.jpg', 'https://m.media-amazon.com/images/I/61qlqvTsocL._SL1664_.jpg', 'https://m.media-amazon.com/images/I/71W6EmfwI-L._SL1664_.jpg', 'https://m.media-amazon.com/images/I/71MllJzfDfL._SL1664_.jpg', 'https://m.media-amazon.com/images/I/71Mwxs8TX+L._SL1664_.jpg', 'https://m.media-amazon.com/images/I/71V25H7JYBL._SL1664_.jpg']</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
           <t>Acer Aspire 3 A325-45 (UN.344SI.004) Laptop (Intel Celeron Dual Core/8 GB/512 GB SSD/Windows 11)</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="K2" t="inlineStr">
         <is>
           <t>Acer</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="L2" t="inlineStr">
         <is>
           <t>A325-45 (UN.344SI.004)</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="M2" t="inlineStr">
         <is>
           <t>Aspire 3</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="N2" t="inlineStr">
         <is>
           <t>17.7 Millimeter thickness</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="O2" t="inlineStr">
         <is>
           <t>357.4 x 228 x 17.7  mm</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
+      <c r="P2" t="inlineStr">
         <is>
           <t>1.5 Kg weight</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
+      <c r="Q2" t="inlineStr">
         <is>
           <t>Silver</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
+      <c r="R2" t="inlineStr">
         <is>
           <t>Windows 11 Home Basic</t>
         </is>
       </c>
-      <c r="O2" t="inlineStr">
+      <c r="S2" t="inlineStr">
         <is>
           <t>64-bit</t>
         </is>
       </c>
-      <c r="P2" t="inlineStr">
+      <c r="T2" t="inlineStr">
         <is>
           <t>15.6 Inches (39.62 cm)</t>
         </is>
       </c>
-      <c r="Q2" t="inlineStr">
+      <c r="U2" t="inlineStr">
         <is>
           <t>1366 x 768 Pixels</t>
         </is>
       </c>
-      <c r="R2" t="inlineStr">
+      <c r="V2" t="inlineStr">
         <is>
           <t>100 ppi</t>
         </is>
       </c>
-      <c r="S2" t="inlineStr">
+      <c r="W2" t="inlineStr">
         <is>
           <t>TN Display With HD
 Acer ComfyView LED-Backlit TFT LCD
@@ -1760,182 +1815,182 @@
 Environment Friendly</t>
         </is>
       </c>
-      <c r="T2" t="inlineStr">
+      <c r="X2" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="U2" t="inlineStr">
+      <c r="Y2" t="inlineStr">
         <is>
           <t>16:9</t>
         </is>
       </c>
-      <c r="V2" t="inlineStr">
+      <c r="Z2" t="inlineStr">
         <is>
           <t>Intel Celeron Dual Core - N4500</t>
         </is>
       </c>
-      <c r="W2" t="inlineStr">
+      <c r="AA2" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="X2" t="inlineStr">
+      <c r="AB2" t="inlineStr">
         <is>
           <t>Intel UHD</t>
         </is>
       </c>
-      <c r="Y2" t="inlineStr">
+      <c r="AC2" t="inlineStr">
         <is>
           <t>8 GB</t>
         </is>
       </c>
-      <c r="Z2" t="inlineStr">
+      <c r="AD2" t="inlineStr">
         <is>
           <t>LPDDR4X</t>
         </is>
       </c>
-      <c r="AA2" t="inlineStr">
+      <c r="AE2" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="AB2" t="inlineStr">
+      <c r="AF2" t="inlineStr">
         <is>
           <t>8 GB</t>
         </is>
       </c>
-      <c r="AC2" t="inlineStr">
+      <c r="AG2" t="inlineStr">
         <is>
           <t>1*8 Gigabyte</t>
         </is>
       </c>
-      <c r="AD2" t="inlineStr">
+      <c r="AH2" t="inlineStr">
         <is>
           <t>512 GB</t>
         </is>
       </c>
-      <c r="AE2" t="inlineStr">
+      <c r="AI2" t="inlineStr">
         <is>
           <t>2 Cell</t>
         </is>
       </c>
-      <c r="AF2" t="inlineStr">
+      <c r="AJ2" t="inlineStr">
         <is>
           <t>Li-Ion</t>
         </is>
       </c>
-      <c r="AG2" t="inlineStr">
+      <c r="AK2" t="inlineStr">
         <is>
           <t>24 W</t>
         </is>
       </c>
-      <c r="AH2" t="inlineStr">
+      <c r="AL2" t="inlineStr">
         <is>
           <t>38 WHrs</t>
         </is>
       </c>
-      <c r="AI2" t="inlineStr">
+      <c r="AM2" t="inlineStr">
         <is>
           <t>802.11 a/b/g/n/ac</t>
         </is>
       </c>
-      <c r="AJ2" t="inlineStr">
+      <c r="AN2" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="AK2" t="inlineStr">
+      <c r="AO2" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="AL2" t="inlineStr">
+      <c r="AP2" t="inlineStr">
         <is>
           <t>5.0</t>
         </is>
       </c>
-      <c r="AM2" t="inlineStr">
+      <c r="AQ2" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="AN2" t="inlineStr">
+      <c r="AR2" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="AO2" t="inlineStr">
+      <c r="AS2" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="AP2" t="inlineStr">
+      <c r="AT2" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="AQ2" t="inlineStr">
+      <c r="AU2" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="AR2" t="inlineStr">
+      <c r="AV2" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="AS2" t="inlineStr">
+      <c r="AW2" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="AT2" t="inlineStr">
+      <c r="AX2" t="inlineStr">
         <is>
           <t>720p</t>
         </is>
       </c>
-      <c r="AU2" t="inlineStr">
+      <c r="AY2" t="inlineStr">
         <is>
           <t>Stereo</t>
         </is>
       </c>
-      <c r="AV2" t="inlineStr">
+      <c r="AZ2" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="AW2" t="inlineStr">
+      <c r="BA2" t="inlineStr">
         <is>
           <t>Built In Microphone</t>
         </is>
       </c>
-      <c r="AX2" t="inlineStr">
+      <c r="BB2" t="inlineStr">
         <is>
           <t>Multi-Gesture Touchpad</t>
         </is>
       </c>
-      <c r="AY2" t="inlineStr">
+      <c r="BC2" t="inlineStr">
         <is>
           <t>95Key Acer Keyboard Layout With International Language Support Including Indicators of CapsLock and F3/Microphone Mute</t>
         </is>
       </c>
-      <c r="AZ2" t="inlineStr">
+      <c r="BD2" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="BA2" t="inlineStr">
+      <c r="BE2" t="inlineStr">
         <is>
           <t>1 Year</t>
         </is>
       </c>
-      <c r="BB2" t="inlineStr">
+      <c r="BF2" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="BC2" t="inlineStr">
+      <c r="BG2" t="inlineStr">
         <is>
           <t>Laptop, Power Adapter, User Manual, Warranty Card</t>
         </is>

</xml_diff>

<commit_message>
feat: Add unique ID extraction and ASIN-based search for Amazon scraper
- Added logic to extract unique product IDs:
  - Flipkart: Extracts 12-character unique ID after 'itm' in the URL.
  - Amazon: Extracts 10-character unique ID after 'dp/' in the URL.

- Updated Amazon scraper:
  - Amazon search now supports ASIN (Amazon Standard Identification Number) as a search query.
  - Ensured product links are filtered and validated.

- Improved search logic:
  - Retained existing product title matching logic using 'span.a-size-medium' and 'a.a-link-normal.s-line-clamp-4'.
  - Enhanced fallback mechanism for finding product links.

- Deduplication:
  - Ensures product links remain unique by converting to a set before returning.

- Logging:
  - Added detailed logs for successful matches, warnings, and errors.
</commit_message>
<xml_diff>
--- a/data/output_scraper_results.xlsx
+++ b/data/output_scraper_results.xlsx
@@ -795,7 +795,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>['https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/x/h/l/-original-imagzk3kcpg6fzxf.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/o/x/n/-original-imagzk3kuu8kduxk.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/d/u/y/-original-imagzk3kukhhjdhq.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/3/j/a/z2-493-thin-and-light-laptop-acer-original-imagr6yjpmhhmpvm.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/l/u/v/z2-493-thin-and-light-laptop-acer-original-imagr6yjuvhjntcb.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/v/t/b/-original-imagvkpfbpgzzqfe.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/a/i/i/-original-imagzk3kfk6bktha.jpeg?q=100&amp;crop=false']</t>
+          <t>['https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/l/u/v/z2-493-thin-and-light-laptop-acer-original-imagr6yjuvhjntcb.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/o/x/n/-original-imagzk3kuu8kduxk.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/a/i/i/-original-imagzk3kfk6bktha.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/d/u/y/-original-imagzk3kukhhjdhq.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/3/j/a/z2-493-thin-and-light-laptop-acer-original-imagr6yjpmhhmpvm.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/v/t/b/-original-imagvkpfbpgzzqfe.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/x/h/l/-original-imagzk3kcpg6fzxf.jpeg?q=100&amp;crop=false']</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -1097,7 +1097,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>['https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/f/w/y/a3sp14-31pt-thin-and-light-laptop-acer-original-imah4bj3ggcejgxd.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/i/n/p/a3sp14-31pt-thin-and-light-laptop-acer-original-imah4bj3jtt5ht8g.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/p/j/o/a3sp14-31pt-thin-and-light-laptop-acer-original-imah4bj3vxnbzuzx.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/g/f/r/a3sp14-31pt-thin-and-light-laptop-acer-original-imah4bj3b5edadhw.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/x/u/3/a3sp14-31pt-thin-and-light-laptop-acer-original-imah4bj3kzhphypa.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/z/m/n/a3sp14-31pt-thin-and-light-laptop-acer-original-imah4bj3v9f9uqff.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/i/2/e/a3sp14-31pt-thin-and-light-laptop-acer-original-imah4bj3zty7uwzt.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/q/j/a/a3sp14-31pt-thin-and-light-laptop-acer-original-imah4bj3nvfzgk9g.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/d/p/j/-original-imagwkaymfh66hw3.jpeg?q=100&amp;crop=false']</t>
+          <t>['https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/g/f/r/a3sp14-31pt-thin-and-light-laptop-acer-original-imah4bj3b5edadhw.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/x/u/3/a3sp14-31pt-thin-and-light-laptop-acer-original-imah4bj3kzhphypa.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/i/n/p/a3sp14-31pt-thin-and-light-laptop-acer-original-imah4bj3jtt5ht8g.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/p/j/o/a3sp14-31pt-thin-and-light-laptop-acer-original-imah4bj3vxnbzuzx.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/f/w/y/a3sp14-31pt-thin-and-light-laptop-acer-original-imah4bj3ggcejgxd.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/i/2/e/a3sp14-31pt-thin-and-light-laptop-acer-original-imah4bj3zty7uwzt.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/q/j/a/a3sp14-31pt-thin-and-light-laptop-acer-original-imah4bj3nvfzgk9g.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/d/p/j/-original-imagwkaymfh66hw3.jpeg?q=100&amp;crop=false', 'https://rukminim2.flixcart.com/image/1664/1664/xif0q/computer/z/m/n/a3sp14-31pt-thin-and-light-laptop-acer-original-imah4bj3v9f9uqff.jpeg?q=100&amp;crop=false']</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -1312,7 +1312,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1351,6 +1351,11 @@
           <t>91 Link</t>
         </is>
       </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Asin</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -1368,14 +1373,14 @@
           <t>Laptop</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>https://www.amazon.in/Acer-Celeron-Processor-LPDDR4X-A325-45/dp/B0D7PYTTGH</t>
-        </is>
-      </c>
       <c r="F2" t="inlineStr">
         <is>
           <t>https://www.91mobiles.com/acer-a325-45-un-344si-004-intel-celeron-dual-core-8-gb-512-gb-windows-11-laptop-price-in-india-163983</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>B0D7PYTTGH</t>
         </is>
       </c>
     </row>
@@ -1718,17 +1723,17 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
+          <t>Acer Aspire 3 Laptop Intel Core Celeron N4500 Processor Laptop (8 GB LPDDR4X SDRAM/512 GB SSD/Win11 Home/38 WHR/HD Webcam) A325-45 with 39.63 cm (15.6") HD Display, Pure Silver, 1.5 KG : Amazon.in: Electronics</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
           <t>NA</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>Acer Aspire 3 Laptop Intel Core Celeron N4500 Processor Laptop (8 GB LPDDR4X SDRAM/512 GB SSD/Win11 Home/38 WHR/HD Webcam) A325-45 with 39.63 cm (15.6") HD Display, Pure Silver, 1.5 KG : Amazon.in: Electronics</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -1738,7 +1743,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>['https://m.media-amazon.com/images/I/71p+Rn+JgbL._SL1664_.jpg', 'https://m.media-amazon.com/images/I/61qlqvTsocL._SL1664_.jpg', 'https://m.media-amazon.com/images/I/71W6EmfwI-L._SL1664_.jpg', 'https://m.media-amazon.com/images/I/71MllJzfDfL._SL1664_.jpg', 'https://m.media-amazon.com/images/I/71Mwxs8TX+L._SL1664_.jpg', 'https://m.media-amazon.com/images/I/71V25H7JYBL._SL1664_.jpg']</t>
+          <t>['https://m.media-amazon.com/images/I/71Mwxs8TX+L._SL1664_.jpg', 'https://m.media-amazon.com/images/I/71W6EmfwI-L._SL1664_.jpg', 'https://m.media-amazon.com/images/I/61qlqvTsocL._SL1664_.jpg', 'https://m.media-amazon.com/images/I/71V25H7JYBL._SL1664_.jpg', 'https://m.media-amazon.com/images/I/71MllJzfDfL._SL1664_.jpg', 'https://m.media-amazon.com/images/I/71p+Rn+JgbL._SL1664_.jpg']</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">

</xml_diff>